<commit_message>
converted data_download from jupyter notebook to .py script
</commit_message>
<xml_diff>
--- a/data/data_financials/ADBE_Balance.xlsx
+++ b/data/data_financials/ADBE_Balance.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -83,7 +83,6 @@
     <col min="8" max="8" bestFit="1" customWidth="1" width="15.400000000000002"/>
     <col min="9" max="9" bestFit="1" customWidth="1" width="15.400000000000002"/>
     <col min="10" max="10" bestFit="1" customWidth="1" width="15.400000000000002"/>
-    <col min="11" max="11" bestFit="1" customWidth="1" width="15.400000000000002"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -119,9 +118,6 @@
       <c r="J1" s="2">
         <v>39780.0</v>
       </c>
-      <c r="K1" s="2">
-        <v>39416.0</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
@@ -156,9 +152,6 @@
       <c r="J2" s="0" t="n">
         <v>886450000.0</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <v>946422000.0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
@@ -193,9 +186,6 @@
       <c r="J3" s="0" t="n">
         <v>1132752000.0</v>
       </c>
-      <c r="K3" s="0" t="n">
-        <v>1047432000.0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
@@ -230,9 +220,6 @@
       <c r="J4" s="0" t="n">
         <v>467234000.0</v>
       </c>
-      <c r="K4" s="0" t="n">
-        <v>318145000.0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
@@ -267,9 +254,6 @@
       <c r="J5" s="0" t="n">
         <v>0.0</v>
       </c>
-      <c r="K5" s="0" t="n">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
@@ -304,9 +288,6 @@
       <c r="J6" s="0" t="n">
         <v>2735103000.0</v>
       </c>
-      <c r="K6" s="0" t="n">
-        <v>2572851000.0</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
@@ -341,9 +322,6 @@
       <c r="J7" s="0" t="n">
         <v>313037000.0</v>
       </c>
-      <c r="K7" s="0" t="n">
-        <v>289758000.0</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
@@ -378,9 +356,6 @@
       <c r="J8" s="0" t="n">
         <v>2349690000.0</v>
       </c>
-      <c r="K8" s="0" t="n">
-        <v>2515746000.0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
@@ -415,9 +390,6 @@
       <c r="J9" s="0" t="n">
         <v>207239000.0</v>
       </c>
-      <c r="K9" s="0" t="n">
-        <v>207239000.0</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
@@ -452,9 +424,6 @@
       <c r="J10" s="0" t="n">
         <v>110713000.0</v>
       </c>
-      <c r="K10" s="0" t="n">
-        <v>171472000.0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
@@ -489,9 +458,6 @@
       <c r="J11" s="0" t="n">
         <v>3086495000.0</v>
       </c>
-      <c r="K11" s="0" t="n">
-        <v>3140828000.0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
@@ -526,9 +492,6 @@
       <c r="J12" s="0" t="n">
         <v>5821598000.0</v>
       </c>
-      <c r="K12" s="0" t="n">
-        <v>5713679000.0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
@@ -563,9 +526,6 @@
       <c r="J13" s="0" t="n">
         <v>55840000.0</v>
       </c>
-      <c r="K13" s="0" t="n">
-        <v>41724000.0</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
@@ -600,9 +560,6 @@
       <c r="J14" s="0" t="n">
         <v>0.0</v>
       </c>
-      <c r="K14" s="0" t="n">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
@@ -637,9 +594,6 @@
       <c r="J15" s="0" t="n">
         <v>762599000.0</v>
       </c>
-      <c r="K15" s="0" t="n">
-        <v>852410000.0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
@@ -674,9 +628,6 @@
       <c r="J16" s="0" t="n">
         <v>350000000.0</v>
       </c>
-      <c r="K16" s="0" t="n">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
@@ -711,9 +662,6 @@
       <c r="J17" s="0" t="n">
         <v>275320000.0</v>
       </c>
-      <c r="K17" s="0" t="n">
-        <v>209268000.0</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
@@ -748,9 +696,6 @@
       <c r="J18" s="0" t="n">
         <v>267646000.0</v>
       </c>
-      <c r="K18" s="0" t="n">
-        <v>364001000.0</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
@@ -785,9 +730,6 @@
       <c r="J19" s="0" t="n">
         <v>0.0</v>
       </c>
-      <c r="K19" s="0" t="n">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
@@ -822,9 +764,6 @@
       <c r="J20" s="0" t="n">
         <v>648645000.0</v>
       </c>
-      <c r="K20" s="0" t="n">
-        <v>211287000.0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
@@ -859,9 +798,6 @@
       <c r="J21" s="0" t="n">
         <v>1411244000.0</v>
       </c>
-      <c r="K21" s="0" t="n">
-        <v>1063697000.0</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
@@ -896,9 +832,6 @@
       <c r="J22" s="0" t="n">
         <v>57222000.0</v>
       </c>
-      <c r="K22" s="0" t="n">
-        <v>27948000.0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
@@ -933,9 +866,6 @@
       <c r="J23" s="0" t="n">
         <v>4913406000.0</v>
       </c>
-      <c r="K23" s="0" t="n">
-        <v>4041592000.0</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
@@ -970,9 +900,6 @@
       <c r="J24" s="0" t="n">
         <v>4410354000.0</v>
       </c>
-      <c r="K24" s="0" t="n">
-        <v>4649982000.0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
@@ -1007,9 +934,6 @@
       <c r="J25" s="0" t="n">
         <v>1339991000.0</v>
       </c>
-      <c r="K25" s="0" t="n">
-        <v>1254671000.0</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
@@ -1044,9 +968,6 @@
       <c r="J26" s="0" t="n">
         <v>350000000.0</v>
       </c>
-      <c r="K26" s="0" t="n">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
@@ -1080,9 +1001,6 @@
       </c>
       <c r="J27" s="0" t="n">
         <v>2019202000.0</v>
-      </c>
-      <c r="K27" s="0" t="n">
-        <v>1993854000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>